<commit_message>
Atualização do arquivo de entrada.
</commit_message>
<xml_diff>
--- a/dados/Tabela de Equivalências_DEER.xlsx
+++ b/dados/Tabela de Equivalências_DEER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\2_Var\Professor\___Pesquisa\Projetos\20230318_Aproveitamentos_Disciplinas_Novo_PPC\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C094182-F2FC-4A0C-BB6D-7B3CC7BB8727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29808F5-B9DD-4403-B2D4-CA1C2CFC418A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{924E8421-3486-4637-9452-14CE2A110864}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{924E8421-3486-4637-9452-14CE2A110864}"/>
   </bookViews>
   <sheets>
     <sheet name="PPC Anterior" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="163">
   <si>
     <t>Disciplina</t>
   </si>
@@ -262,9 +262,6 @@
     <t>Materiais Elétricos</t>
   </si>
   <si>
-    <t>Tópicos Avançados em Engenharia de Energias Renováveis</t>
-  </si>
-  <si>
     <t>Tópicos Especiais em Engenharia de Energias Renováveis I</t>
   </si>
   <si>
@@ -518,6 +515,21 @@
   </si>
   <si>
     <t>Optativa 9°</t>
+  </si>
+  <si>
+    <t>Tópicos Avançados em Engenharia de Energias Renováveis I</t>
+  </si>
+  <si>
+    <t>Tópicos Avançados em Engenharia de Energias Renováveis II</t>
+  </si>
+  <si>
+    <t>Tópicos Avançados em Engenharia de Energias Renováveis III</t>
+  </si>
+  <si>
+    <t>Tópicos Avançados em Engenharia de Energias Renováveis IV</t>
+  </si>
+  <si>
+    <t>Flexíveis</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724857A3-A0BE-491E-B865-A0646934EAE1}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1049,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1046,12 +1058,12 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
@@ -1066,7 +1078,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>6</v>
@@ -1081,7 +1093,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>10</v>
@@ -1096,7 +1108,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
@@ -1111,7 +1123,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>9</v>
@@ -1126,10 +1138,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="9">
         <v>60</v>
@@ -1141,10 +1153,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="9">
         <v>60</v>
@@ -1156,7 +1168,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>5</v>
@@ -1171,10 +1183,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C10" s="9">
         <v>60</v>
@@ -1186,10 +1198,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="9">
         <v>75</v>
@@ -1202,7 +1214,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>12</v>
@@ -1217,7 +1229,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>13</v>
@@ -1232,7 +1244,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>14</v>
@@ -1247,10 +1259,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="9">
         <v>45</v>
@@ -1262,7 +1274,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>17</v>
@@ -1277,7 +1289,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>18</v>
@@ -1292,7 +1304,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>20</v>
@@ -1307,7 +1319,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>19</v>
@@ -1322,7 +1334,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>3</v>
@@ -1337,7 +1349,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>8</v>
@@ -1352,7 +1364,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>21</v>
@@ -1367,10 +1379,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" s="9">
         <v>45</v>
@@ -1382,7 +1394,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>23</v>
@@ -1397,7 +1409,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>27</v>
@@ -1412,10 +1424,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="9">
         <v>60</v>
@@ -1427,7 +1439,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>28</v>
@@ -1442,10 +1454,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C28" s="9">
         <v>60</v>
@@ -1457,10 +1469,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29" s="9">
         <v>60</v>
@@ -1472,10 +1484,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C30" s="9">
         <v>60</v>
@@ -1487,7 +1499,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>31</v>
@@ -1502,7 +1514,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>24</v>
@@ -1517,7 +1529,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>33</v>
@@ -1532,7 +1544,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>32</v>
@@ -1547,7 +1559,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>34</v>
@@ -1562,7 +1574,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>30</v>
@@ -1577,7 +1589,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>36</v>
@@ -1592,7 +1604,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>62</v>
@@ -1607,10 +1619,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C39" s="9">
         <v>60</v>
@@ -1622,7 +1634,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>39</v>
@@ -1637,7 +1649,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>40</v>
@@ -1652,7 +1664,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>41</v>
@@ -1667,7 +1679,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>2</v>
@@ -1682,7 +1694,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>43</v>
@@ -1697,10 +1709,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C45" s="9">
         <v>60</v>
@@ -1712,10 +1724,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C46" s="9">
         <v>75</v>
@@ -1727,7 +1739,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>47</v>
@@ -1742,7 +1754,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>60</v>
@@ -1757,7 +1769,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>45</v>
@@ -1772,7 +1784,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>42</v>
@@ -1787,7 +1799,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>54</v>
@@ -1802,10 +1814,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C52" s="9">
         <v>90</v>
@@ -1817,10 +1829,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" s="9">
         <v>30</v>
@@ -1832,10 +1844,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" s="9">
         <v>60</v>
@@ -1847,7 +1859,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>52</v>
@@ -1862,7 +1874,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>61</v>
@@ -1877,10 +1889,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C57" s="9">
         <v>60</v>
@@ -1892,10 +1904,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58" s="9">
         <v>90</v>
@@ -1907,10 +1919,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C59" s="9">
         <v>60</v>
@@ -1922,10 +1934,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60" s="9">
         <v>60</v>
@@ -1937,7 +1949,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>48</v>
@@ -1952,10 +1964,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C62" s="9">
         <v>30</v>
@@ -1967,7 +1979,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>58</v>
@@ -1982,10 +1994,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C64" s="9">
         <v>180</v>
@@ -1997,7 +2009,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>63</v>
+        <v>162</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>63</v>
@@ -2012,7 +2024,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>56</v>
@@ -2027,7 +2039,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>66</v>
@@ -2042,7 +2054,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>72</v>
@@ -2057,7 +2069,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>67</v>
@@ -2072,7 +2084,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>22</v>
@@ -2087,7 +2099,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>70</v>
@@ -2102,7 +2114,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>65</v>
@@ -2117,7 +2129,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>64</v>
@@ -2132,7 +2144,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>68</v>
@@ -2147,7 +2159,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>69</v>
@@ -2162,7 +2174,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>71</v>
@@ -2177,10 +2189,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C77" s="9">
         <v>60</v>
@@ -2192,10 +2204,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C78" s="9">
         <v>30</v>
@@ -2207,10 +2219,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C79" s="9">
         <v>30</v>
@@ -2222,10 +2234,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C80" s="9">
         <v>30</v>
@@ -2243,16 +2255,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE2BA82-CD6A-45D0-8E13-65807E8DCBA0}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A57" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -2260,7 +2272,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -2269,15 +2281,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
@@ -2295,7 +2307,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>6</v>
@@ -2313,7 +2325,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>10</v>
@@ -2331,7 +2343,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
@@ -2349,7 +2361,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>9</v>
@@ -2367,7 +2379,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>8</v>
@@ -2385,10 +2397,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="9">
         <v>60</v>
@@ -2403,7 +2415,7 @@
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>5</v>
@@ -2421,10 +2433,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C10" s="9">
         <v>60</v>
@@ -2439,7 +2451,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>12</v>
@@ -2457,7 +2469,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>13</v>
@@ -2475,7 +2487,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>14</v>
@@ -2493,10 +2505,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" s="9">
         <v>60</v>
@@ -2511,7 +2523,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>16</v>
@@ -2529,7 +2541,7 @@
     </row>
     <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>17</v>
@@ -2547,7 +2559,7 @@
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>18</v>
@@ -2565,7 +2577,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>20</v>
@@ -2583,7 +2595,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>19</v>
@@ -2601,7 +2613,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>3</v>
@@ -2619,7 +2631,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>22</v>
@@ -2637,7 +2649,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>21</v>
@@ -2655,10 +2667,10 @@
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="9">
         <v>60</v>
@@ -2673,7 +2685,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>27</v>
@@ -2691,7 +2703,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>24</v>
@@ -2709,7 +2721,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>29</v>
@@ -2727,7 +2739,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>26</v>
@@ -2745,10 +2757,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="9">
         <v>60</v>
@@ -2763,10 +2775,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="9">
         <v>30</v>
@@ -2781,10 +2793,10 @@
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="9">
         <v>60</v>
@@ -2799,7 +2811,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>33</v>
@@ -2817,7 +2829,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>32</v>
@@ -2835,7 +2847,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>34</v>
@@ -2853,10 +2865,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="9">
         <v>60</v>
@@ -2871,10 +2883,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="9">
         <v>30</v>
@@ -2889,10 +2901,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36" s="9">
         <v>30</v>
@@ -2907,7 +2919,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>35</v>
@@ -2925,7 +2937,7 @@
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>36</v>
@@ -2943,10 +2955,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="9">
         <v>60</v>
@@ -2961,7 +2973,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>38</v>
@@ -2979,7 +2991,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>39</v>
@@ -2997,10 +3009,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="9">
         <v>60</v>
@@ -3015,7 +3027,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>40</v>
@@ -3033,7 +3045,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>41</v>
@@ -3051,10 +3063,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="9">
         <v>30</v>
@@ -3069,7 +3081,7 @@
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>47</v>
@@ -3087,10 +3099,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C47" s="9">
         <v>60</v>
@@ -3105,7 +3117,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>42</v>
@@ -3123,7 +3135,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>46</v>
@@ -3141,7 +3153,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>44</v>
@@ -3159,10 +3171,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" s="9">
         <v>60</v>
@@ -3177,10 +3189,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C52" s="9">
         <v>60</v>
@@ -3195,10 +3207,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C53" s="9">
         <v>60</v>
@@ -3213,10 +3225,10 @@
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" s="9">
         <v>30</v>
@@ -3231,7 +3243,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>53</v>
@@ -3249,7 +3261,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>50</v>
@@ -3267,7 +3279,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>51</v>
@@ -3285,7 +3297,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>48</v>
@@ -3303,10 +3315,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C59" s="9">
         <v>60</v>
@@ -3321,10 +3333,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C60" s="9">
         <v>30</v>
@@ -3339,10 +3351,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C61" s="9">
         <v>30</v>
@@ -3357,10 +3369,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C62" s="9">
         <v>30</v>
@@ -3375,10 +3387,10 @@
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C63" s="9">
         <v>60</v>
@@ -3393,7 +3405,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>57</v>
@@ -3411,7 +3423,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>59</v>
@@ -3429,7 +3441,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>2</v>
@@ -3447,7 +3459,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>55</v>
@@ -3465,7 +3477,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>60</v>
@@ -3483,10 +3495,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C69" s="9">
         <v>30</v>
@@ -3501,10 +3513,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70" s="9">
         <v>30</v>
@@ -3519,10 +3531,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C71" s="9">
         <v>60</v>
@@ -3537,10 +3549,10 @@
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C72" s="9">
         <v>180</v>
@@ -3555,7 +3567,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>61</v>
@@ -3573,10 +3585,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C74" s="9">
         <v>30</v>
@@ -3591,10 +3603,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C75" s="9">
         <v>30</v>
@@ -3609,7 +3621,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>63</v>
+        <v>162</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>63</v>
@@ -3627,16 +3639,16 @@
     </row>
     <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B77" s="8" t="s">
-        <v>95</v>
-      </c>
       <c r="C77" s="9">
         <v>30</v>
       </c>
       <c r="D77" s="9">
-        <f t="shared" ref="D77:D99" si="2">C77/15</f>
+        <f t="shared" ref="D77:D102" si="2">C77/15</f>
         <v>2</v>
       </c>
       <c r="E77" s="9">
@@ -3645,10 +3657,10 @@
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C78" s="9">
         <v>30</v>
@@ -3663,10 +3675,10 @@
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C79" s="9">
         <v>30</v>
@@ -3681,7 +3693,7 @@
     </row>
     <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>68</v>
@@ -3699,7 +3711,7 @@
     </row>
     <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>69</v>
@@ -3717,10 +3729,10 @@
     </row>
     <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C82" s="9">
         <v>30</v>
@@ -3735,10 +3747,10 @@
     </row>
     <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C83" s="9">
         <v>30</v>
@@ -3753,10 +3765,10 @@
     </row>
     <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C84" s="9">
         <v>30</v>
@@ -3771,7 +3783,7 @@
     </row>
     <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>66</v>
@@ -3789,10 +3801,10 @@
     </row>
     <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C86" s="9">
         <v>30</v>
@@ -3807,7 +3819,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>71</v>
@@ -3825,10 +3837,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C88" s="9">
         <v>30</v>
@@ -3843,10 +3855,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C89" s="9">
         <v>30</v>
@@ -3861,10 +3873,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C90" s="9">
         <v>30</v>
@@ -3879,7 +3891,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>65</v>
@@ -3897,7 +3909,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>64</v>
@@ -3915,7 +3927,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>67</v>
@@ -3933,10 +3945,10 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C94" s="9">
         <v>30</v>
@@ -3951,7 +3963,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>70</v>
@@ -3969,10 +3981,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C96" s="16">
         <v>30</v>
@@ -3987,10 +3999,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C97" s="9">
         <v>30</v>
@@ -4005,10 +4017,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="C98" s="9">
         <v>30</v>
@@ -4023,19 +4035,73 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>108</v>
+        <v>159</v>
       </c>
       <c r="C99" s="9">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D99" s="9">
+        <f t="shared" ref="D99:D101" si="3">C99/15</f>
+        <v>2</v>
+      </c>
+      <c r="E99" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C100" s="9">
+        <v>30</v>
+      </c>
+      <c r="D100" s="9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E100" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C101" s="9">
+        <v>30</v>
+      </c>
+      <c r="D101" s="9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E101" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C102" s="9">
+        <v>60</v>
+      </c>
+      <c r="D102" s="9">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E99" s="9">
+      <c r="E102" s="9">
         <v>0</v>
       </c>
     </row>
@@ -4048,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F37B09A-964C-4DC6-815A-03183FF59EA3}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4063,19 +4129,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>129</v>
-      </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4182,7 +4248,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" s="1">
         <v>90</v>
@@ -4216,13 +4282,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="1">
         <v>60</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" s="1">
         <v>60</v>
@@ -4301,13 +4367,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" s="1">
         <v>135</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D15" s="1">
         <v>120</v>
@@ -4443,7 +4509,7 @@
         <v>90</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D23" s="1">
         <v>90</v>
@@ -4460,7 +4526,7 @@
         <v>90</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24" s="1">
         <v>120</v>
@@ -4528,7 +4594,7 @@
         <v>90</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D28" s="1">
         <v>120</v>
@@ -4545,7 +4611,7 @@
         <v>90</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D29" s="1">
         <v>120</v>
@@ -4596,7 +4662,7 @@
         <v>60</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D32" s="1">
         <v>60</v>
@@ -4607,7 +4673,7 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B33" s="1">
         <v>90</v>
@@ -4641,13 +4707,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="1">
         <v>60</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D35" s="1">
         <v>60</v>
@@ -4698,7 +4764,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D38" s="1">
         <v>90</v>
@@ -4715,7 +4781,7 @@
         <v>90</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D39" s="1">
         <v>90</v>
@@ -4760,13 +4826,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" s="1">
         <v>60</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D42" s="1">
         <v>60</v>
@@ -4777,13 +4843,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B43" s="1">
         <v>30</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D43" s="1">
         <v>30</v>
@@ -4828,7 +4894,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B46" s="1">
         <v>90</v>
@@ -4845,13 +4911,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B47" s="1">
         <v>60</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D47" s="1">
         <v>60</v>
@@ -4998,7 +5064,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B56" s="1">
         <v>60</v>
@@ -5021,7 +5087,7 @@
         <v>60</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D57" s="1">
         <v>30</v>
@@ -5032,7 +5098,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B58" s="26">
         <v>60</v>
@@ -5049,13 +5115,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B59" s="1">
         <v>180</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D59" s="1">
         <v>180</v>
@@ -5219,13 +5285,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B69" s="1">
         <v>60</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D69" s="1">
         <v>60</v>
@@ -5242,7 +5308,7 @@
         <v>45</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="D70" s="26">
         <v>30</v>
@@ -5253,13 +5319,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71" s="26">
         <v>30</v>
       </c>
       <c r="C71" s="25" t="s">
-        <v>73</v>
+        <v>159</v>
       </c>
       <c r="D71" s="26">
         <v>30</v>
@@ -5270,13 +5336,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" s="26">
         <v>30</v>
       </c>
       <c r="C72" s="25" t="s">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="D72" s="26">
         <v>30</v>
@@ -5287,13 +5353,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73" s="26">
         <v>30</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="D73" s="26">
         <v>30</v>

</xml_diff>

<commit_message>
Atualização da tabela de equivalências
</commit_message>
<xml_diff>
--- a/dados/Tabela de Equivalências_DEER.xlsx
+++ b/dados/Tabela de Equivalências_DEER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\2_Var\Professor\___Pesquisa\Projetos\20230318_Aproveitamentos_Disciplinas_Novo_PPC\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F97BDE-1CB8-4C4B-8ABC-FEF565A5D01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD73868-28D6-45A2-B91F-C95FD97F9F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{924E8421-3486-4637-9452-14CE2A110864}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{924E8421-3486-4637-9452-14CE2A110864}"/>
   </bookViews>
   <sheets>
     <sheet name="PPC Anterior" sheetId="3" r:id="rId1"/>
@@ -120,9 +120,6 @@
     <t>Química Orgânica para Tecnólogos</t>
   </si>
   <si>
-    <t xml:space="preserve">Química Orgânica Teórica A </t>
-  </si>
-  <si>
     <t>Termodinâmica II</t>
   </si>
   <si>
@@ -499,6 +496,9 @@
   </si>
   <si>
     <t>Sistemas Elétricos Aplicados* &amp;&amp; Laboratório de Circuitos Elétricos*</t>
+  </si>
+  <si>
+    <t>Fundamentos de Físico-Química</t>
   </si>
 </sst>
 </file>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724857A3-A0BE-491E-B865-A0646934EAE1}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1003,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1012,12 +1012,12 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -1026,13 +1026,13 @@
         <v>60</v>
       </c>
       <c r="D2" s="7">
-        <f>C2/15</f>
+        <f t="shared" ref="D2:D33" si="0">C2/15</f>
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>6</v>
@@ -1041,16 +1041,16 @@
         <v>60</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" ref="D3:D59" si="0">C3/15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>108</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="7">
         <v>60</v>
@@ -1062,10 +1062,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>108</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="C5" s="7">
         <v>60</v>
@@ -1077,10 +1077,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>9</v>
+        <v>108</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="C6" s="7">
         <v>60</v>
@@ -1092,37 +1092,37 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>96</v>
+        <v>108</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="C7" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="C8" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>5</v>
@@ -1137,37 +1137,37 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="C10" s="7">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="C11" s="7">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
@@ -1182,22 +1182,22 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="C13" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>14</v>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="7">
         <v>45</v>
@@ -1227,10 +1227,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C16" s="7">
         <v>60</v>
@@ -1242,10 +1242,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="7">
         <v>60</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" s="7">
         <v>60</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>18</v>
@@ -1287,10 +1287,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C20" s="7">
         <v>60</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>8</v>
@@ -1317,55 +1317,55 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C22" s="7">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D22" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="C23" s="7">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D23" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="C24" s="7">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D24" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C25" s="7">
         <v>60</v>
@@ -1377,10 +1377,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C26" s="7">
         <v>60</v>
@@ -1392,25 +1392,25 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C27" s="7">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D27" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="7">
         <v>60</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C29" s="7">
         <v>60</v>
@@ -1437,10 +1437,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="C30" s="7">
         <v>60</v>
@@ -1452,10 +1452,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C31" s="7">
         <v>90</v>
@@ -1467,172 +1467,172 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C32" s="7">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="D32" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="C33" s="7">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D33" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
       <c r="C34" s="7">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D34" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" ref="D34:D65" si="1">C34/15</f>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35" s="7">
         <v>60</v>
       </c>
       <c r="D35" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C36" s="7">
         <v>90</v>
       </c>
       <c r="D36" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C37" s="7">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D37" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="C38" s="7">
         <v>60</v>
       </c>
       <c r="D38" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="C39" s="7">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C40" s="7">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C41" s="7">
         <v>75</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C42" s="7">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>2</v>
@@ -1641,271 +1641,271 @@
         <v>45</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C44" s="7">
         <v>60</v>
       </c>
       <c r="D44" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>69</v>
+        <v>114</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C45" s="7">
         <v>60</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="7">
         <v>75</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C47" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D47" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>52</v>
+        <v>114</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C48" s="7">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D48" s="7">
-        <f>C48/15</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>37</v>
+        <v>114</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C49" s="7">
         <v>60</v>
       </c>
       <c r="D49" s="7">
-        <f>C49/15</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>34</v>
+        <v>114</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C50" s="7">
         <v>30</v>
       </c>
       <c r="D50" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="C51" s="7">
         <v>60</v>
       </c>
       <c r="D51" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="C52" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D52" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C53" s="7">
         <v>60</v>
       </c>
       <c r="D53" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C54" s="7">
         <v>45</v>
       </c>
       <c r="D54" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C55" s="7">
         <v>30</v>
       </c>
       <c r="D55" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="C56" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D56" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C57" s="7">
         <v>60</v>
       </c>
       <c r="D57" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C58" s="7">
         <v>60</v>
       </c>
       <c r="D58" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C59" s="7">
         <v>30</v>
       </c>
       <c r="D59" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="C60" s="7">
         <v>30</v>
       </c>
       <c r="D60" s="7">
-        <f t="shared" ref="D60:D63" si="1">C60/15</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="C61" s="7">
         <v>30</v>
@@ -1917,10 +1917,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C62" s="7">
         <v>180</v>
@@ -1932,10 +1932,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C63" s="7">
         <v>90</v>
@@ -1947,22 +1947,22 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C64" s="7">
         <v>45</v>
       </c>
       <c r="D64" s="7">
-        <f t="shared" ref="D64:D74" si="2">C64/15</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>58</v>
@@ -1971,31 +1971,31 @@
         <v>45</v>
       </c>
       <c r="D65" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C66" s="7">
         <v>45</v>
       </c>
       <c r="D66" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D66:D97" si="2">C66/15</f>
         <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C67" s="7">
         <v>45</v>
@@ -2007,37 +2007,37 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>140</v>
+        <v>61</v>
       </c>
       <c r="C68" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D68" s="7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C69" s="7">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D69" s="7">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>57</v>
@@ -2052,25 +2052,25 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="C71" s="7">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D71" s="7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="C72" s="7">
         <v>45</v>
@@ -2082,10 +2082,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C73" s="7">
         <v>45</v>
@@ -2097,10 +2097,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C74" s="7">
         <v>45</v>
@@ -2112,66 +2112,71 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="C75" s="7">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D75" s="7">
-        <f t="shared" ref="D75:D76" si="3">C75/15</f>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C76" s="7">
         <v>30</v>
       </c>
       <c r="D76" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C77" s="7">
         <v>30</v>
       </c>
       <c r="D77" s="7">
-        <f t="shared" ref="D77:D78" si="4">C77/15</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C78" s="7">
         <v>30</v>
       </c>
       <c r="D78" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D78" xr:uid="{724857A3-A0BE-491E-B865-A0646934EAE1}"/>
+  <autoFilter ref="A1:D78" xr:uid="{724857A3-A0BE-491E-B865-A0646934EAE1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D78">
+      <sortCondition ref="A2:A78"/>
+      <sortCondition ref="B2:B78"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -2181,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE2BA82-CD6A-45D0-8E13-65807E8DCBA0}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="B76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,7 +2201,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -2205,15 +2210,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -2222,7 +2227,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="7">
-        <f>C2/15</f>
+        <f t="shared" ref="D2:D31" si="0">C2/15</f>
         <v>4</v>
       </c>
       <c r="E2" s="7">
@@ -2231,7 +2236,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>6</v>
@@ -2240,7 +2245,7 @@
         <v>60</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" ref="D3:D59" si="0">C3/15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E3" s="7">
@@ -2249,10 +2254,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>108</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="7">
         <v>60</v>
@@ -2262,15 +2267,15 @@
         <v>4</v>
       </c>
       <c r="E4" s="7">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C5" s="7">
         <v>60</v>
@@ -2280,51 +2285,51 @@
         <v>4</v>
       </c>
       <c r="E5" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>9</v>
+        <v>108</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" s="7">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="C7" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="7">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>141</v>
+        <v>7</v>
       </c>
       <c r="C8" s="7">
         <v>60</v>
@@ -2334,33 +2339,33 @@
         <v>4</v>
       </c>
       <c r="E8" s="7">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="C10" s="7">
         <v>60</v>
@@ -2375,10 +2380,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C11" s="7">
         <v>60</v>
@@ -2388,33 +2393,33 @@
         <v>4</v>
       </c>
       <c r="E11" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D12" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" s="7">
         <v>60</v>
@@ -2424,15 +2429,15 @@
         <v>4</v>
       </c>
       <c r="E13" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="C14" s="7">
         <v>60</v>
@@ -2442,15 +2447,15 @@
         <v>4</v>
       </c>
       <c r="E14" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="7">
         <v>60</v>
@@ -2460,15 +2465,15 @@
         <v>4</v>
       </c>
       <c r="E15" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C16" s="7">
         <v>60</v>
@@ -2478,15 +2483,15 @@
         <v>4</v>
       </c>
       <c r="E16" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="7">
         <v>60</v>
@@ -2501,10 +2506,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" s="7">
         <v>60</v>
@@ -2514,15 +2519,15 @@
         <v>4</v>
       </c>
       <c r="E18" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C19" s="7">
         <v>30</v>
@@ -2537,10 +2542,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C20" s="7">
         <v>60</v>
@@ -2550,15 +2555,15 @@
         <v>4</v>
       </c>
       <c r="E20" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21" s="7">
         <v>60</v>
@@ -2573,10 +2578,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C22" s="7">
         <v>60</v>
@@ -2586,15 +2591,15 @@
         <v>4</v>
       </c>
       <c r="E22" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="C23" s="7">
         <v>60</v>
@@ -2609,28 +2614,28 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C24" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D24" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E24" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="C25" s="7">
         <v>60</v>
@@ -2640,15 +2645,15 @@
         <v>4</v>
       </c>
       <c r="E25" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="C26" s="7">
         <v>60</v>
@@ -2663,10 +2668,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>22</v>
+        <v>135</v>
       </c>
       <c r="C27" s="7">
         <v>60</v>
@@ -2681,10 +2686,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="C28" s="7">
         <v>60</v>
@@ -2699,10 +2704,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>145</v>
+        <v>23</v>
       </c>
       <c r="C29" s="7">
         <v>60</v>
@@ -2717,10 +2722,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>26</v>
+        <v>142</v>
       </c>
       <c r="C30" s="7">
         <v>60</v>
@@ -2735,10 +2740,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" s="7">
         <v>60</v>
@@ -2753,16 +2758,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>27</v>
+        <v>151</v>
       </c>
       <c r="C32" s="7">
         <v>30</v>
       </c>
       <c r="D32" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D32:D65" si="1">C32/15</f>
         <v>2</v>
       </c>
       <c r="E32" s="7">
@@ -2771,17 +2776,17 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>143</v>
+        <v>26</v>
       </c>
       <c r="C33" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D33" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E33" s="7">
         <v>4</v>
@@ -2789,17 +2794,17 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C34" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D34" s="7">
-        <f t="shared" ref="D34" si="1">C34/15</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E34" s="7">
         <v>4</v>
@@ -2807,16 +2812,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C35" s="7">
         <v>60</v>
       </c>
       <c r="D35" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E35" s="7">
@@ -2825,17 +2830,17 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="C36" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D36" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E36" s="7">
         <v>4</v>
@@ -2843,16 +2848,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="C37" s="7">
         <v>60</v>
       </c>
       <c r="D37" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E37" s="7">
@@ -2861,16 +2866,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="7">
         <v>60</v>
       </c>
       <c r="D38" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E38" s="7">
@@ -2879,7 +2884,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>32</v>
@@ -2888,7 +2893,7 @@
         <v>60</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E39" s="7">
@@ -2897,17 +2902,17 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>142</v>
+        <v>28</v>
       </c>
       <c r="C40" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E40" s="7">
         <v>4</v>
@@ -2915,16 +2920,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="C41" s="7">
         <v>60</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E41" s="7">
@@ -2933,16 +2938,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="C42" s="7">
         <v>60</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E42" s="7">
@@ -2951,17 +2956,17 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>39</v>
+        <v>113</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="C43" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E43" s="7">
         <v>4</v>
@@ -2969,16 +2974,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>146</v>
+        <v>37</v>
       </c>
       <c r="C44" s="7">
         <v>60</v>
       </c>
       <c r="D44" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E44" s="7">
@@ -2987,17 +2992,17 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>34</v>
+        <v>114</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="C45" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E45" s="7">
         <v>4</v>
@@ -3005,35 +3010,35 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="C46" s="7">
         <v>60</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E46" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>36</v>
+        <v>114</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C47" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D47" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E47" s="7">
         <v>4</v>
@@ -3041,16 +3046,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C48" s="7">
         <v>60</v>
       </c>
       <c r="D48" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E48" s="7">
@@ -3059,53 +3064,53 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C49" s="7">
         <v>60</v>
       </c>
       <c r="D49" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E49" s="7">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>72</v>
+        <v>114</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C50" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D50" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E50" s="7">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="C51" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D51" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E51" s="7">
         <v>4</v>
@@ -3113,17 +3118,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C52" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D52" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E52" s="7">
         <v>4</v>
@@ -3131,16 +3136,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C53" s="7">
         <v>60</v>
       </c>
       <c r="D53" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E53" s="7">
@@ -3149,16 +3154,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="C54" s="7">
         <v>60</v>
       </c>
       <c r="D54" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E54" s="7">
@@ -3167,35 +3172,35 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C55" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D55" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E55" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C56" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D56" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E56" s="7">
         <v>4</v>
@@ -3203,35 +3208,35 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="C57" s="7">
         <v>60</v>
       </c>
       <c r="D57" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E57" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C58" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D58" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E58" s="7">
         <v>4</v>
@@ -3239,35 +3244,35 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="C59" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D59" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E59" s="7">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C60" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D60" s="7">
-        <f t="shared" ref="D60:D65" si="2">C60/15</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E60" s="7">
         <v>4</v>
@@ -3275,52 +3280,52 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C61" s="7">
         <v>30</v>
       </c>
       <c r="D61" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E61" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C62" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D62" s="7">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E62" s="7">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" s="7">
         <v>180</v>
       </c>
       <c r="D63" s="7">
-        <f t="shared" si="2"/>
+        <f>C63/15</f>
         <v>12</v>
       </c>
       <c r="E63" s="7">
@@ -3329,16 +3334,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C64" s="7">
         <v>60</v>
       </c>
       <c r="D64" s="7">
-        <f t="shared" si="2"/>
+        <f>C64/15</f>
         <v>4</v>
       </c>
       <c r="E64" s="7">
@@ -3347,16 +3352,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C65" s="7">
         <v>60</v>
       </c>
       <c r="D65" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E65" s="7">
@@ -3365,7 +3370,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>79</v>
@@ -3374,7 +3379,7 @@
         <v>30</v>
       </c>
       <c r="D66" s="7">
-        <f t="shared" ref="D66:D91" si="3">C66/15</f>
+        <f t="shared" ref="D66:D97" si="2">C66/15</f>
         <v>2</v>
       </c>
       <c r="E66" s="7">
@@ -3383,16 +3388,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="C67" s="7">
         <v>30</v>
       </c>
       <c r="D67" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E67" s="7">
@@ -3401,16 +3406,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C68" s="7">
         <v>30</v>
       </c>
       <c r="D68" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E68" s="7">
@@ -3419,16 +3424,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C69" s="7">
         <v>30</v>
       </c>
       <c r="D69" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E69" s="7">
@@ -3437,16 +3442,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C70" s="7">
         <v>30</v>
       </c>
       <c r="D70" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E70" s="7">
@@ -3455,16 +3460,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C71" s="7">
         <v>30</v>
       </c>
       <c r="D71" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E71" s="7">
@@ -3473,16 +3478,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C72" s="7">
         <v>30</v>
       </c>
       <c r="D72" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E72" s="7">
@@ -3491,16 +3496,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C73" s="7">
         <v>30</v>
       </c>
       <c r="D73" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E73" s="7">
@@ -3509,16 +3514,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="C74" s="7">
         <v>30</v>
       </c>
       <c r="D74" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E74" s="7">
@@ -3527,16 +3532,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="C75" s="7">
         <v>30</v>
       </c>
       <c r="D75" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E75" s="7">
@@ -3545,16 +3550,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C76" s="7">
         <v>30</v>
       </c>
       <c r="D76" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E76" s="7">
@@ -3563,16 +3568,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="C77" s="7">
         <v>30</v>
       </c>
       <c r="D77" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E77" s="7">
@@ -3581,16 +3586,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C78" s="7">
         <v>30</v>
       </c>
       <c r="D78" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E78" s="7">
@@ -3599,7 +3604,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>88</v>
@@ -3608,7 +3613,7 @@
         <v>30</v>
       </c>
       <c r="D79" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E79" s="7">
@@ -3617,16 +3622,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="C80" s="7">
         <v>30</v>
       </c>
       <c r="D80" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E80" s="7">
@@ -3635,16 +3640,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C81" s="7">
         <v>30</v>
       </c>
       <c r="D81" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E81" s="7">
@@ -3653,16 +3658,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="C82" s="7">
         <v>30</v>
       </c>
       <c r="D82" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E82" s="7">
@@ -3671,34 +3676,34 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C83" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D83" s="7">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="E83" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C84" s="7">
         <v>30</v>
       </c>
       <c r="D84" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E84" s="7">
@@ -3707,16 +3712,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="C85" s="14">
         <v>30</v>
       </c>
       <c r="D85" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E85" s="7">
@@ -3725,16 +3730,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C86" s="7">
         <v>30</v>
       </c>
       <c r="D86" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E86" s="7">
@@ -3743,16 +3748,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="C87" s="7">
         <v>30</v>
       </c>
       <c r="D87" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E87" s="7">
@@ -3761,16 +3766,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C88" s="7">
         <v>30</v>
       </c>
       <c r="D88" s="7">
-        <f t="shared" ref="D88:D90" si="4">C88/15</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E88" s="7">
@@ -3779,16 +3784,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C89" s="7">
         <v>30</v>
       </c>
       <c r="D89" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E89" s="7">
@@ -3797,16 +3802,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C90" s="7">
         <v>30</v>
       </c>
       <c r="D90" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E90" s="7">
@@ -3815,24 +3820,29 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="C91" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D91" s="7">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="E91" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E91" xr:uid="{ADE2BA82-CD6A-45D0-8E13-65807E8DCBA0}"/>
+  <autoFilter ref="A1:E91" xr:uid="{ADE2BA82-CD6A-45D0-8E13-65807E8DCBA0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E91">
+      <sortCondition ref="A2:A91"/>
+      <sortCondition ref="B2:B91"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -3841,8 +3851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F37B09A-964C-4DC6-815A-03183FF59EA3}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A68" sqref="A67:B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3853,10 +3863,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3909,7 +3919,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -3925,10 +3935,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3957,18 +3967,18 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -4021,10 +4031,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4032,20 +4042,20 @@
         <v>21</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
@@ -4063,200 +4073,200 @@
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>25</v>
+      <c r="B27" s="21" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -4269,170 +4279,170 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção em Fundamentos de Físico-Química...
</commit_message>
<xml_diff>
--- a/dados/Tabela de Equivalências_DEER.xlsx
+++ b/dados/Tabela de Equivalências_DEER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\2_Var\Professor\___Pesquisa\Projetos\20230318_Aproveitamentos_Disciplinas_Novo_PPC\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD73868-28D6-45A2-B91F-C95FD97F9F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276AE2E1-AE27-426A-8D89-548B9637A431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{924E8421-3486-4637-9452-14CE2A110864}"/>
   </bookViews>
@@ -1986,7 +1986,7 @@
         <v>45</v>
       </c>
       <c r="D66" s="7">
-        <f t="shared" ref="D66:D97" si="2">C66/15</f>
+        <f t="shared" ref="D66:D78" si="2">C66/15</f>
         <v>3</v>
       </c>
     </row>
@@ -2186,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE2BA82-CD6A-45D0-8E13-65807E8DCBA0}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:XFD64"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,11 +2764,11 @@
         <v>151</v>
       </c>
       <c r="C32" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D32" s="7">
         <f t="shared" ref="D32:D65" si="1">C32/15</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E32" s="7">
         <v>4</v>
@@ -3379,7 +3379,7 @@
         <v>30</v>
       </c>
       <c r="D66" s="7">
-        <f t="shared" ref="D66:D97" si="2">C66/15</f>
+        <f t="shared" ref="D66:D91" si="2">C66/15</f>
         <v>2</v>
       </c>
       <c r="E66" s="7">

</xml_diff>